<commit_message>
added test methof for getting activity by UserId
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Activity.xlsx
+++ b/src/test/resources/data/Activity.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NazmulHossain\Projects\external-api-qa\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A75C472-B955-421B-BEDD-8E35893D2E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9720E9-5CEF-4487-92E4-F46D45264EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3570" yWindow="-11865" windowWidth="32565" windowHeight="9030" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
+    <workbookView xWindow="2570" yWindow="0" windowWidth="16630" windowHeight="7550" activeTab="1" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
   </bookViews>
   <sheets>
     <sheet name="GET_activity_v1_users" sheetId="1" r:id="rId1"/>
-    <sheet name="ImpactData_2" sheetId="2" r:id="rId2"/>
+    <sheet name="GET_last_login" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>TCID</t>
   </si>
@@ -77,31 +77,28 @@
     <t>200</t>
   </si>
   <si>
-    <t>400</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
     <t>(Not Supported currently)</t>
   </si>
   <si>
-    <t>Get Module Guide</t>
-  </si>
-  <si>
-    <t>​/impacts​/v1​/impacts​/{moduleGuid}​/comments</t>
-  </si>
-  <si>
     <t>preRequisite</t>
   </si>
   <si>
-    <t>Get Impact by module guide.</t>
-  </si>
-  <si>
     <t>Get User Activity Survey</t>
   </si>
   <si>
     <t>/activity/v1/users?startTimestamp=2020-5-1&amp;endTimestamp=2022-5-1&amp;pageSize=100</t>
+  </si>
+  <si>
+    <t>Get Last Login</t>
+  </si>
+  <si>
+    <t>Get valid userId for Last Login</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/last-logins</t>
   </si>
 </sst>
 </file>
@@ -478,8 +475,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B7E84D1-294A-4626-81FA-9856648E2C09}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -536,19 +533,19 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -580,8 +577,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B88D30-C8DE-42A0-A9E2-8B6287FAD006}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -603,7 +600,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -632,16 +629,16 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
@@ -649,7 +646,7 @@
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -657,72 +654,48 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
-      <c r="E4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
       <c r="G4" s="1"/>
-      <c r="H4" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>17</v>
-      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="J5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added method for getting user sessions
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Activity.xlsx
+++ b/src/test/resources/data/Activity.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NazmulHossain\Projects\external-api-qa\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9720E9-5CEF-4487-92E4-F46D45264EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA467680-452C-475A-8C1D-9821BB2338B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2570" yWindow="0" windowWidth="16630" windowHeight="7550" activeTab="1" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
+    <workbookView xWindow="10845" yWindow="-20850" windowWidth="33900" windowHeight="12675" activeTab="2" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
   </bookViews>
   <sheets>
     <sheet name="GET_activity_v1_users" sheetId="1" r:id="rId1"/>
     <sheet name="GET_last_login" sheetId="2" r:id="rId2"/>
+    <sheet name="GET_user_sessions" sheetId="5" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="22">
   <si>
     <t>TCID</t>
   </si>
@@ -77,9 +78,6 @@
     <t>200</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>(Not Supported currently)</t>
   </si>
   <si>
@@ -95,10 +93,16 @@
     <t>Get Last Login</t>
   </si>
   <si>
-    <t>Get valid userId for Last Login</t>
-  </si>
-  <si>
     <t>/activity/v1/users/{userId}/last-logins</t>
+  </si>
+  <si>
+    <t>Get valid userId from Activity API</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/sessions</t>
+  </si>
+  <si>
+    <t>Get User Sessions</t>
   </si>
 </sst>
 </file>
@@ -533,19 +537,19 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -577,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B88D30-C8DE-42A0-A9E2-8B6287FAD006}">
   <dimension ref="A1:J5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -587,6 +591,9 @@
     <col min="4" max="4" width="43.90625" customWidth="1"/>
     <col min="6" max="6" width="52.6328125" customWidth="1"/>
     <col min="7" max="7" width="13.36328125" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="9" max="9" width="25.81640625" customWidth="1"/>
+    <col min="10" max="10" width="26.1796875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.35">
@@ -600,7 +607,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -629,7 +636,7 @@
         <v>9</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>19</v>
@@ -638,7 +645,7 @@
         <v>7</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1" t="s">
@@ -646,16 +653,12 @@
       </c>
       <c r="I2" s="1"/>
       <c r="J2" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -666,12 +669,8 @@
       <c r="J3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A4" s="2"/>
+      <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -682,20 +681,131 @@
       <c r="J4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
-      <c r="J5" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3388F2-1909-45A3-81C6-E34A543E1DC2}">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="52.26953125" customWidth="1"/>
+    <col min="4" max="4" width="43.90625" customWidth="1"/>
+    <col min="6" max="6" width="52.6328125" customWidth="1"/>
+    <col min="7" max="7" width="13.36328125" customWidth="1"/>
+    <col min="8" max="8" width="22" customWidth="1"/>
+    <col min="9" max="9" width="25.81640625" customWidth="1"/>
+    <col min="10" max="10" width="26.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1"/>
+      <c r="J2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A5" s="2"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added new method to Activity api tests
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Activity.xlsx
+++ b/src/test/resources/data/Activity.xlsx
@@ -8,14 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NazmulHossain\Projects\external-api-qa\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA467680-452C-475A-8C1D-9821BB2338B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57029B92-9376-4000-B18E-F04FA25941A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10845" yWindow="-20850" windowWidth="33900" windowHeight="12675" activeTab="2" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
+    <workbookView xWindow="5370" yWindow="-19515" windowWidth="30165" windowHeight="17520" activeTab="5" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
   </bookViews>
   <sheets>
-    <sheet name="GET_activity_v1_users" sheetId="1" r:id="rId1"/>
-    <sheet name="GET_last_login" sheetId="2" r:id="rId2"/>
-    <sheet name="GET_user_sessions" sheetId="5" r:id="rId3"/>
+    <sheet name="GET_user_simultaneous_logins" sheetId="7" r:id="rId1"/>
+    <sheet name="GET_activity_v1_users" sheetId="1" r:id="rId2"/>
+    <sheet name="GET_last_login" sheetId="2" r:id="rId3"/>
+    <sheet name="GET_user_simultaneous" sheetId="6" r:id="rId4"/>
+    <sheet name="GET_user_sessions" sheetId="5" r:id="rId5"/>
+    <sheet name="GET_user_summary" sheetId="8" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="26">
   <si>
     <t>TCID</t>
   </si>
@@ -48,9 +51,6 @@
     <t>HttpMethod</t>
   </si>
   <si>
-    <t>Body</t>
-  </si>
-  <si>
     <t>Uri</t>
   </si>
   <si>
@@ -103,6 +103,21 @@
   </si>
   <si>
     <t>Get User Sessions</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/simultaneous?startTimestamp=2020-5-1&amp;endTimestamp=2022-5-1</t>
+  </si>
+  <si>
+    <t>Get Simultaneous User Activity</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/simultaneous-logins?startTimestamp=2020-5-1&amp;endTimestamp=2022-5-1</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/{userId}/summary</t>
+  </si>
+  <si>
+    <t>Get User Summary</t>
   </si>
 </sst>
 </file>
@@ -476,98 +491,174 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C3772B-6738-4612-BB2C-6B6DC76D6E13}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="30.1796875" customWidth="1"/>
+    <col min="4" max="4" width="32.7265625" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="6" max="6" width="82.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="8" max="8" width="25.81640625" customWidth="1"/>
+    <col min="9" max="9" width="26.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B7E84D1-294A-4626-81FA-9856648E2C09}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="8.7265625" style="1"/>
-    <col min="3" max="3" width="55.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="31.6328125" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.7265625" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="69.7265625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="21.6328125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="26.1796875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.453125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="26.1796875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.7265625" style="1"/>
+    <col min="6" max="6" width="70.54296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.1796875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="26.1796875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="H1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
     </row>
   </sheetData>
@@ -577,12 +668,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B88D30-C8DE-42A0-A9E2-8B6287FAD006}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -590,73 +681,68 @@
     <col min="3" max="3" width="52.26953125" customWidth="1"/>
     <col min="4" max="4" width="43.90625" customWidth="1"/>
     <col min="6" max="6" width="52.6328125" customWidth="1"/>
-    <col min="7" max="7" width="13.36328125" customWidth="1"/>
-    <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="25.81640625" customWidth="1"/>
-    <col min="10" max="10" width="26.1796875" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="8" max="8" width="25.81640625" customWidth="1"/>
+    <col min="9" max="9" width="26.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="H1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -666,9 +752,8 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -678,16 +763,14 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -695,86 +778,161 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3388F2-1909-45A3-81C6-E34A543E1DC2}">
-  <dimension ref="A1:J5"/>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1505332-9685-449B-8C4A-AB02E3790084}">
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="52.26953125" customWidth="1"/>
+    <col min="3" max="3" width="30.1796875" customWidth="1"/>
+    <col min="4" max="4" width="32.7265625" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="6" max="6" width="82.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="8" max="8" width="25.81640625" customWidth="1"/>
+    <col min="9" max="9" width="26.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3388F2-1909-45A3-81C6-E34A543E1DC2}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="21.54296875" customWidth="1"/>
     <col min="4" max="4" width="43.90625" customWidth="1"/>
     <col min="6" max="6" width="52.6328125" customWidth="1"/>
-    <col min="7" max="7" width="13.36328125" customWidth="1"/>
-    <col min="8" max="8" width="22" customWidth="1"/>
-    <col min="9" max="9" width="25.81640625" customWidth="1"/>
-    <col min="10" max="10" width="26.1796875" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="8" max="8" width="25.81640625" customWidth="1"/>
+    <col min="9" max="9" width="26.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="H1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="3" t="s">
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -784,9 +942,8 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -796,16 +953,124 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{086B76B2-2B82-421F-92E2-E6E040E4DE28}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="21.54296875" customWidth="1"/>
+    <col min="4" max="4" width="43.90625" customWidth="1"/>
+    <col min="6" max="6" width="52.6328125" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="8" max="8" width="25.81640625" customWidth="1"/>
+    <col min="9" max="9" width="26.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="2"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Productivy test methods complete and running
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Activity.xlsx
+++ b/src/test/resources/data/Activity.xlsx
@@ -8,17 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NazmulHossain\Projects\external-api-qa\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57029B92-9376-4000-B18E-F04FA25941A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400D83EE-73E6-4B60-A083-8C97CE57411E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5370" yWindow="-19515" windowWidth="30165" windowHeight="17520" activeTab="5" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
+    <workbookView xWindow="11550" yWindow="-20265" windowWidth="27495" windowHeight="17250" firstSheet="4" activeTab="6" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
   </bookViews>
   <sheets>
-    <sheet name="GET_user_simultaneous_logins" sheetId="7" r:id="rId1"/>
-    <sheet name="GET_activity_v1_users" sheetId="1" r:id="rId2"/>
-    <sheet name="GET_last_login" sheetId="2" r:id="rId3"/>
-    <sheet name="GET_user_simultaneous" sheetId="6" r:id="rId4"/>
+    <sheet name="GET_activity_v1_users" sheetId="1" r:id="rId1"/>
+    <sheet name="GET_last_login" sheetId="2" r:id="rId2"/>
+    <sheet name="GET_user_simultaneous" sheetId="6" r:id="rId3"/>
+    <sheet name="GET_user_simultaneous_logins" sheetId="7" r:id="rId4"/>
     <sheet name="GET_user_sessions" sheetId="5" r:id="rId5"/>
     <sheet name="GET_user_summary" sheetId="8" r:id="rId6"/>
+    <sheet name="GET_equipment" sheetId="9" r:id="rId7"/>
+    <sheet name="GET_equipId_sessions" sheetId="11" r:id="rId8"/>
+    <sheet name="GET_equipId_summary" sheetId="12" r:id="rId9"/>
+    <sheet name="GET_equipId_last_login" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="25">
   <si>
     <t>TCID</t>
   </si>
@@ -67,9 +71,6 @@
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>preRequisites</t>
   </si>
   <si>
     <t>FieldValidations</t>
@@ -491,6 +492,306 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B7E84D1-294A-4626-81FA-9856648E2C09}">
+  <dimension ref="A1:I6"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="2" width="8.7265625" style="1"/>
+    <col min="3" max="3" width="31.6328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7265625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="70.54296875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="26.1796875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="17.453125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="26.1796875" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="2"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ACB6C26-1AE1-43B2-8661-B07D21F9446D}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B88D30-C8DE-42A0-A9E2-8B6287FAD006}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="52.26953125" customWidth="1"/>
+    <col min="4" max="4" width="43.90625" customWidth="1"/>
+    <col min="6" max="6" width="52.6328125" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="8" max="8" width="25.81640625" customWidth="1"/>
+    <col min="9" max="9" width="26.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="2"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="2"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1505332-9685-449B-8C4A-AB02E3790084}">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="30.1796875" customWidth="1"/>
+    <col min="4" max="4" width="32.7265625" customWidth="1"/>
+    <col min="5" max="5" width="12.81640625" customWidth="1"/>
+    <col min="6" max="6" width="82.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22" customWidth="1"/>
+    <col min="8" max="8" width="25.81640625" customWidth="1"/>
+    <col min="9" max="9" width="26.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1"/>
+      <c r="I2" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C3772B-6738-4612-BB2C-6B6DC76D6E13}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -520,7 +821,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -532,7 +833,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>5</v>
@@ -546,311 +847,23 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B7E84D1-294A-4626-81FA-9856648E2C09}">
-  <dimension ref="A1:I6"/>
-  <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="2" width="8.7265625" style="1"/>
-    <col min="3" max="3" width="31.6328125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7265625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="70.54296875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.1796875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.453125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="26.1796875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B88D30-C8DE-42A0-A9E2-8B6287FAD006}">
-  <dimension ref="A1:I5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="3" max="3" width="52.26953125" customWidth="1"/>
-    <col min="4" max="4" width="43.90625" customWidth="1"/>
-    <col min="6" max="6" width="52.6328125" customWidth="1"/>
-    <col min="7" max="7" width="22" customWidth="1"/>
-    <col min="8" max="8" width="25.81640625" customWidth="1"/>
-    <col min="9" max="9" width="26.1796875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1505332-9685-449B-8C4A-AB02E3790084}">
-  <dimension ref="A1:I2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="3" max="3" width="30.1796875" customWidth="1"/>
-    <col min="4" max="4" width="32.7265625" customWidth="1"/>
-    <col min="5" max="5" width="12.81640625" customWidth="1"/>
-    <col min="6" max="6" width="82.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22" customWidth="1"/>
-    <col min="8" max="8" width="25.81640625" customWidth="1"/>
-    <col min="9" max="9" width="26.1796875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -887,7 +900,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -899,7 +912,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>5</v>
@@ -913,23 +926,23 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -972,7 +985,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{086B76B2-2B82-421F-92E2-E6E040E4DE28}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -997,7 +1010,7 @@
         <v>1</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>2</v>
@@ -1009,7 +1022,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>5</v>
@@ -1023,23 +1036,23 @@
         <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
@@ -1076,4 +1089,42 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9FFDFA5-5332-432A-9925-5010622BDC15}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9AE10D00-541A-4267-9151-85470916DD6A}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7F63CBE-20C6-4938-94A8-B06668624B57}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added ReadMe for how to run the tests
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Activity.xlsx
+++ b/src/test/resources/data/Activity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NazmulHossain\Projects\external-api-qa\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{400D83EE-73E6-4B60-A083-8C97CE57411E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6611C4F-41A0-4EF7-A5B1-3EB0A1D52DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11550" yWindow="-20265" windowWidth="27495" windowHeight="17250" firstSheet="4" activeTab="6" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
+    <workbookView xWindow="4380" yWindow="-19305" windowWidth="27120" windowHeight="17925" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
   </bookViews>
   <sheets>
     <sheet name="GET_activity_v1_users" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="34">
   <si>
     <t>TCID</t>
   </si>
@@ -119,6 +119,33 @@
   </si>
   <si>
     <t>Get User Summary</t>
+  </si>
+  <si>
+    <t>Get User Activity without startTimeStamp param</t>
+  </si>
+  <si>
+    <t>/activity/v1/users?endTimestamp=2022-5-1&amp;pageSize=100</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>Get User Activity without endTimeStamp param</t>
+  </si>
+  <si>
+    <t>/activity/v1/users?startTimestamp=2020-5-1&amp;pageSize=100</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Get User Activity without pageSize param</t>
+  </si>
+  <si>
+    <t>PageSize is listed as a mandatory query on swagger but by default the server will provide a fault pageSIze if one is not provided by the client</t>
+  </si>
+  <si>
+    <t>/activity/v1/users?startTimestamp=2020-5-1&amp;endTimestamp=2022-5-1</t>
   </si>
 </sst>
 </file>
@@ -173,11 +200,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -493,26 +521,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B7E84D1-294A-4626-81FA-9856648E2C09}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="2" width="8.7265625" style="1"/>
-    <col min="3" max="3" width="31.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="45" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.7265625" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="70.54296875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="26.1796875" style="1" customWidth="1"/>
-    <col min="8" max="8" width="17.453125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="73.7265625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.36328125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="22.6328125" style="1" customWidth="1"/>
     <col min="9" max="9" width="26.1796875" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="1"/>
+    <col min="10" max="10" width="19.90625" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -540,8 +569,11 @@
       <c r="I1" s="3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="J1" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -560,26 +592,77 @@
       <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
       <c r="I2" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
     </row>
   </sheetData>
@@ -1095,7 +1178,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9FFDFA5-5332-432A-9925-5010622BDC15}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>

</xml_diff>

<commit_message>
added new test cases and updated Readme
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Activity.xlsx
+++ b/src/test/resources/data/Activity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NazmulHossain\Projects\external-api-qa\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6611C4F-41A0-4EF7-A5B1-3EB0A1D52DE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3E0B1F-A7A8-4540-95F6-CAE659BB6146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="-19305" windowWidth="27120" windowHeight="17925" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
+    <workbookView xWindow="4380" yWindow="-19305" windowWidth="27120" windowHeight="17925" activeTab="1" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
   </bookViews>
   <sheets>
     <sheet name="GET_activity_v1_users" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="36">
   <si>
     <t>TCID</t>
   </si>
@@ -146,6 +146,12 @@
   </si>
   <si>
     <t>/activity/v1/users?startTimestamp=2020-5-1&amp;endTimestamp=2022-5-1</t>
+  </si>
+  <si>
+    <t>Get Last login with invalid userId</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/a416e744-c66f-48b1-af78-055aa30aa982/last-logins</t>
   </si>
 </sst>
 </file>
@@ -523,8 +529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B7E84D1-294A-4626-81FA-9856648E2C09}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -688,8 +694,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B88D30-C8DE-42A0-A9E2-8B6287FAD006}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -759,13 +765,25 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>27</v>
+      </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added schema validation for the activity survey endpoint
</commit_message>
<xml_diff>
--- a/src/test/resources/data/Activity.xlsx
+++ b/src/test/resources/data/Activity.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NazmulHossain\Projects\external-api-qa\src\test\resources\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA3E0B1F-A7A8-4540-95F6-CAE659BB6146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{455673B3-C438-49D7-BABD-3B4FB2800B7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4380" yWindow="-19305" windowWidth="27120" windowHeight="17925" activeTab="1" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" xr2:uid="{04B38584-319A-4E31-822B-CD2CB9389256}"/>
   </bookViews>
   <sheets>
     <sheet name="GET_activity_v1_users" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="43">
   <si>
     <t>TCID</t>
   </si>
@@ -152,6 +152,27 @@
   </si>
   <si>
     <t>/activity/v1/users/a416e744-c66f-48b1-af78-055aa30aa982/last-logins</t>
+  </si>
+  <si>
+    <t>Get Simultaneous User Activity with Invalid UserId</t>
+  </si>
+  <si>
+    <t>Get User Activity with pageSize=1</t>
+  </si>
+  <si>
+    <t>/activity/v1/users?startTimestamp=2020-5-1&amp;endTimestamp=2022-5-1&amp;pageSize=1</t>
+  </si>
+  <si>
+    <t>/activity/v1/users/a416e744-c66f-48b1-af78-055aa30aa982/simultaneous?startTimestamp=2020-5-1&amp;endTimestamp=2022-5-1</t>
+  </si>
+  <si>
+    <t>schemaValidationFile</t>
+  </si>
+  <si>
+    <t>getActivitySurvey.json</t>
+  </si>
+  <si>
+    <t>400error.json</t>
   </si>
 </sst>
 </file>
@@ -527,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B7E84D1-294A-4626-81FA-9856648E2C09}">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -539,15 +560,14 @@
     <col min="3" max="3" width="45" style="1" customWidth="1"/>
     <col min="4" max="4" width="14.7265625" style="1" customWidth="1"/>
     <col min="5" max="5" width="11.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="73.7265625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="50.26953125" style="1" customWidth="1"/>
     <col min="7" max="7" width="19.36328125" style="1" customWidth="1"/>
     <col min="8" max="8" width="22.6328125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="26.1796875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="19.90625" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="8.7265625" style="1"/>
+    <col min="9" max="9" width="19.90625" style="1" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -570,16 +590,13 @@
         <v>4</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>9</v>
+        <v>40</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="J1" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -598,14 +615,11 @@
       <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H2" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -624,8 +638,11 @@
       <c r="G3" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H3" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -644,8 +661,11 @@
       <c r="G4" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="H4" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -664,12 +684,35 @@
       <c r="G5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="H5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I5" s="4" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A6" s="2"/>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -694,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3B88D30-C8DE-42A0-A9E2-8B6287FAD006}">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -814,18 +857,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1505332-9685-449B-8C4A-AB02E3790084}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="30.1796875" customWidth="1"/>
+    <col min="3" max="3" width="42.26953125" customWidth="1"/>
     <col min="4" max="4" width="32.7265625" customWidth="1"/>
     <col min="5" max="5" width="12.81640625" customWidth="1"/>
-    <col min="6" max="6" width="82.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="67.08984375" customWidth="1"/>
     <col min="7" max="7" width="22" customWidth="1"/>
     <col min="8" max="8" width="25.81640625" customWidth="1"/>
     <col min="9" max="9" width="26.1796875" customWidth="1"/>
@@ -887,6 +930,31 @@
         <v>11</v>
       </c>
     </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -897,7 +965,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>